<commit_message>
ihm/serie_3 and serie_4 finished
</commit_message>
<xml_diff>
--- a/Moyennes_DUT.xlsx
+++ b/Moyennes_DUT.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\azkil\BARTHO\Code\iut\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A94E917E-FE45-4B8D-ADA1-D3FE46710EE0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DBCBEDF-6FAB-4F47-8F86-33256C8587AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="300" windowWidth="29040" windowHeight="16020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1291,7 +1291,7 @@
   <dimension ref="A1:R100"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1647,7 +1647,7 @@
         <v>2.5</v>
       </c>
       <c r="H11" s="11">
-        <v>13</v>
+        <v>12.8</v>
       </c>
       <c r="I11" s="12"/>
       <c r="J11" s="16" t="s">
@@ -1731,7 +1731,7 @@
       </c>
       <c r="H13" s="21">
         <f>(H3*G3+H4*G4+H5*G5+H6*G6+H7*G7+H8*G8+H9*G9+H10*G10+H11*G11+H12*G12)/G13</f>
-        <v>12.5721875</v>
+        <v>12.5409375</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="9" t="s">
@@ -1992,7 +1992,7 @@
         <v>2.5</v>
       </c>
       <c r="H20" s="11">
-        <v>16</v>
+        <v>15.6</v>
       </c>
       <c r="I20" s="2"/>
       <c r="J20" s="28" t="s">
@@ -2063,7 +2063,7 @@
       </c>
       <c r="H22" s="33">
         <f>(H14*G14+H15*G15+H16*G16+H17*G17+H18*G18+H19*G19+H20*G20+H21*G21)/G22</f>
-        <v>11.142857142857142</v>
+        <v>11.071428571428571</v>
       </c>
       <c r="I22" s="2"/>
       <c r="J22" s="34" t="s">
@@ -2145,7 +2145,7 @@
       </c>
       <c r="G25" s="45">
         <f>(H13*G13+H22*G22)/F25</f>
-        <v>11.905166666666666</v>
+        <v>11.855166666666666</v>
       </c>
       <c r="H25" s="46"/>
       <c r="I25" s="2"/>
@@ -2190,7 +2190,7 @@
       <c r="A27" s="2"/>
       <c r="B27" s="41">
         <f>(C25+G25)/2</f>
-        <v>13.715833333333334</v>
+        <v>13.690833333333334</v>
       </c>
       <c r="C27" s="44"/>
       <c r="D27" s="44"/>
@@ -2231,7 +2231,7 @@
       <c r="A29" s="2"/>
       <c r="B29" s="41">
         <f>(B27+J27)/2</f>
-        <v>6.8579166666666671</v>
+        <v>6.8454166666666669</v>
       </c>
       <c r="C29" s="42"/>
       <c r="D29" s="42"/>

</xml_diff>

<commit_message>
feat: s4/prog_rep thread tps
</commit_message>
<xml_diff>
--- a/Moyennes_DUT.xlsx
+++ b/Moyennes_DUT.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\azkil\BARTHO\Code\iut\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEE793EC-1A7B-41D0-9730-220C11E5803A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34C1016A-C915-416D-89B8-FB1DD2AC84AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="70">
   <si>
     <t>S1</t>
   </si>
@@ -63,9 +63,6 @@
     <t>SE TP</t>
   </si>
   <si>
-    <t>C++</t>
-  </si>
-  <si>
     <t>Init Lin</t>
   </si>
   <si>
@@ -93,9 +90,6 @@
     <t>PHP</t>
   </si>
   <si>
-    <t>Cloud comp</t>
-  </si>
-  <si>
     <t>Algo 2</t>
   </si>
   <si>
@@ -238,6 +232,15 @@
   </si>
   <si>
     <t>Algo Avancé</t>
+  </si>
+  <si>
+    <t>Prog répartie</t>
+  </si>
+  <si>
+    <t>Entreprise</t>
+  </si>
+  <si>
+    <t>V</t>
   </si>
 </sst>
 </file>
@@ -308,7 +311,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -668,11 +671,82 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -780,6 +854,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1194,8 +1283,8 @@
   </sheetPr>
   <dimension ref="A1:R100"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="O23" sqref="O23"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1211,33 +1300,33 @@
     <col min="17" max="16384" width="14.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:16" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="39" t="s">
+    <row r="1" spans="2:17" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:17" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="41"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="46"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="39" t="s">
+      <c r="F2" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="42"/>
-      <c r="H2" s="41"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="46"/>
       <c r="I2" s="2"/>
-      <c r="J2" s="39" t="s">
+      <c r="J2" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="42"/>
-      <c r="L2" s="41"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="46"/>
       <c r="M2" s="2"/>
-      <c r="N2" s="39" t="s">
+      <c r="N2" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="O2" s="42"/>
-      <c r="P2" s="41"/>
-    </row>
-    <row r="3" spans="2:16" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O2" s="47"/>
+      <c r="P2" s="46"/>
+    </row>
+    <row r="3" spans="2:17" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
@@ -1274,11 +1363,11 @@
       <c r="O3" s="7">
         <v>1.5</v>
       </c>
-      <c r="P3" s="8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="2:16" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P3" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:17" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="s">
         <v>7</v>
       </c>
@@ -1310,18 +1399,18 @@
       </c>
       <c r="M4" s="2"/>
       <c r="N4" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="O4" s="10">
+        <v>1.5</v>
+      </c>
+      <c r="P4" s="40">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="2:17" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="9" t="s">
         <v>10</v>
-      </c>
-      <c r="O4" s="10">
-        <v>1.25</v>
-      </c>
-      <c r="P4" s="8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="2:16" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="9" t="s">
-        <v>11</v>
       </c>
       <c r="C5" s="10">
         <v>1</v>
@@ -1331,7 +1420,7 @@
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G5" s="10">
         <v>1</v>
@@ -1351,18 +1440,18 @@
       </c>
       <c r="M5" s="2"/>
       <c r="N5" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="O5" s="10">
+        <v>1.5</v>
+      </c>
+      <c r="P5" s="40">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="9" t="s">
         <v>13</v>
-      </c>
-      <c r="O5" s="10">
-        <v>1.25</v>
-      </c>
-      <c r="P5" s="8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="2:16" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="9" t="s">
-        <v>14</v>
       </c>
       <c r="C6" s="10">
         <v>1.7</v>
@@ -1372,7 +1461,7 @@
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G6" s="10">
         <v>2.5</v>
@@ -1382,7 +1471,7 @@
       </c>
       <c r="I6" s="12"/>
       <c r="J6" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="K6" s="10">
         <v>1.5</v>
@@ -1392,18 +1481,18 @@
       </c>
       <c r="M6" s="2"/>
       <c r="N6" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="O6" s="10">
+        <v>1.5</v>
+      </c>
+      <c r="P6" s="40">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="9" t="s">
         <v>16</v>
-      </c>
-      <c r="O6" s="10">
-        <v>1.25</v>
-      </c>
-      <c r="P6" s="8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="2:16" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="9" t="s">
-        <v>17</v>
       </c>
       <c r="C7" s="10">
         <v>1.8</v>
@@ -1413,7 +1502,7 @@
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G7" s="10">
         <v>1.25</v>
@@ -1423,7 +1512,7 @@
       </c>
       <c r="I7" s="12"/>
       <c r="J7" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K7" s="10">
         <v>1.5</v>
@@ -1433,18 +1522,18 @@
       </c>
       <c r="M7" s="2"/>
       <c r="N7" s="9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O7" s="10">
         <v>0.75</v>
       </c>
-      <c r="P7" s="8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="2:16" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P7" s="40">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="2:17" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C8" s="10">
         <v>1.2</v>
@@ -1454,7 +1543,7 @@
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G8" s="10">
         <v>1.25</v>
@@ -1464,7 +1553,7 @@
       </c>
       <c r="I8" s="12"/>
       <c r="J8" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="K8" s="10">
         <v>1</v>
@@ -1474,18 +1563,18 @@
       </c>
       <c r="M8" s="2"/>
       <c r="N8" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="O8" s="10">
         <v>0.75</v>
       </c>
-      <c r="P8" s="8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="2:16" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P8" s="40">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C9" s="10">
         <v>1.3</v>
@@ -1495,7 +1584,7 @@
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G9" s="10">
         <v>1</v>
@@ -1505,7 +1594,7 @@
       </c>
       <c r="I9" s="12"/>
       <c r="J9" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="K9" s="10">
         <v>2.5</v>
@@ -1515,18 +1604,21 @@
       </c>
       <c r="M9" s="2"/>
       <c r="N9" s="9" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="O9" s="10">
-        <v>0.75</v>
-      </c>
-      <c r="P9" s="8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="2:16" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.5</v>
+      </c>
+      <c r="P9" s="42">
+        <v>14.5</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C10" s="10">
         <v>1.7</v>
@@ -1536,7 +1628,7 @@
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G10" s="10">
         <v>1.5</v>
@@ -1546,7 +1638,7 @@
       </c>
       <c r="I10" s="12"/>
       <c r="J10" s="13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="K10" s="14">
         <v>1.5</v>
@@ -1555,19 +1647,21 @@
         <v>14.25</v>
       </c>
       <c r="M10" s="2"/>
-      <c r="N10" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="O10" s="10">
-        <v>2.5</v>
-      </c>
-      <c r="P10" s="8">
+      <c r="N10" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="O10" s="41">
+        <f>O3+O4+O5+O6+O7+O8+O9</f>
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="2:16" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P10" s="43">
+        <f>(P3*O3+O4*P4+O5*P5+P6*O6+P7*O7+P8*O8+P9*O9)/O10</f>
+        <v>13.3</v>
+      </c>
+    </row>
+    <row r="11" spans="2:17" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C11" s="10">
         <v>1.8</v>
@@ -1577,7 +1671,7 @@
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G11" s="10">
         <v>2.5</v>
@@ -1587,7 +1681,7 @@
       </c>
       <c r="I11" s="12"/>
       <c r="J11" s="16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="K11" s="17">
         <f>K3+K4+K5+K6+K7+K8+K9+K10</f>
@@ -1598,21 +1692,19 @@
         <v>14.681666666666667</v>
       </c>
       <c r="M11" s="2"/>
-      <c r="N11" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="O11" s="17">
-        <f>O3+O4+O5+O6+O7+O8+O9+O10</f>
-        <v>10</v>
-      </c>
-      <c r="P11" s="18">
-        <f>(P3*O3+O4*P4+O5*P5+P6*O6+P7*O7+P8*O8+P9*O9+P10*O10)/O11</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="2:16" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N11" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="O11" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="P11" s="5">
+        <v>14.83</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C12" s="10">
         <v>1.7</v>
@@ -1622,7 +1714,7 @@
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G12" s="14">
         <v>2</v>
@@ -1632,7 +1724,7 @@
       </c>
       <c r="I12" s="12"/>
       <c r="J12" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="K12" s="4">
         <v>2.5</v>
@@ -1642,18 +1734,18 @@
       </c>
       <c r="M12" s="2"/>
       <c r="N12" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="O12" s="4">
         <v>1.5</v>
       </c>
       <c r="P12" s="5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="2:16" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="2:17" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C13" s="10">
         <v>0.8</v>
@@ -1663,7 +1755,7 @@
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="19" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G13" s="20">
         <f>G3+G4+G5+G6+G7+G8+G9+G10+G11+G12</f>
@@ -1675,7 +1767,7 @@
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="K13" s="10">
         <v>1.5</v>
@@ -1685,19 +1777,19 @@
         <v>10.1</v>
       </c>
       <c r="M13" s="2"/>
-      <c r="N13" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="O13" s="4">
-        <v>1.5</v>
+      <c r="N13" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="O13" s="10">
+        <v>2</v>
       </c>
       <c r="P13" s="5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="2:16" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="2:17" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C14" s="14">
         <v>1.5</v>
@@ -1707,7 +1799,7 @@
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="22" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G14" s="23">
         <v>2.5</v>
@@ -1717,7 +1809,7 @@
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K14" s="10">
         <v>1.5</v>
@@ -1727,18 +1819,18 @@
       </c>
       <c r="M14" s="2"/>
       <c r="N14" s="9" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="O14" s="10">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="P14" s="5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="2:16" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="2:17" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="16" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C15" s="17">
         <f>C3+C4+C5+C6+C7+C8+C9+C10+C11+C12+C13+C14</f>
@@ -1750,7 +1842,7 @@
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G15" s="10">
         <v>2</v>
@@ -1760,7 +1852,7 @@
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="K15" s="10">
         <v>2.5</v>
@@ -1770,18 +1862,18 @@
       </c>
       <c r="M15" s="2"/>
       <c r="N15" s="9" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="O15" s="10">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="P15" s="5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="2:16" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>14.25</v>
+      </c>
+    </row>
+    <row r="16" spans="2:17" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C16" s="4">
         <v>2.5</v>
@@ -1791,7 +1883,7 @@
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G16" s="4">
         <v>3</v>
@@ -1801,7 +1893,7 @@
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K16" s="10">
         <v>1.5</v>
@@ -1811,20 +1903,20 @@
       </c>
       <c r="M16" s="2"/>
       <c r="N16" s="16" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="O16" s="17">
-        <f>O12+O13+O14+O15</f>
+        <f>O11+O12+O13+O14+O15</f>
         <v>8</v>
       </c>
       <c r="P16" s="18">
-        <f>(P13*O13+P14*O14+P15*O15+P12*O12)/O16</f>
-        <v>10</v>
+        <f>(P12*O12+P13*O13+P14*O14+P11*O11+P15*O15)/O16</f>
+        <v>14.624375000000001</v>
       </c>
     </row>
     <row r="17" spans="1:18" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C17" s="10">
         <v>2</v>
@@ -1834,7 +1926,7 @@
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G17" s="10">
         <v>0.75</v>
@@ -1844,7 +1936,7 @@
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="13" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K17" s="14">
         <v>2.5</v>
@@ -1854,7 +1946,7 @@
       </c>
       <c r="M17" s="2"/>
       <c r="N17" s="16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="O17" s="26">
         <v>12</v>
@@ -1865,7 +1957,7 @@
     </row>
     <row r="18" spans="1:18" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C18" s="10">
         <v>1.5</v>
@@ -1875,7 +1967,7 @@
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G18" s="10">
         <v>0.75</v>
@@ -1885,7 +1977,7 @@
       </c>
       <c r="I18" s="2"/>
       <c r="J18" s="16" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K18" s="17">
         <f>+K12+K13+K14+K15+K16+K17</f>
@@ -1902,7 +1994,7 @@
     </row>
     <row r="19" spans="1:18" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C19" s="10">
         <v>2.5</v>
@@ -1912,7 +2004,7 @@
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G19" s="10">
         <v>1.5</v>
@@ -1922,7 +2014,7 @@
       </c>
       <c r="I19" s="2"/>
       <c r="J19" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K19" s="4">
         <v>1.8</v>
@@ -1937,7 +2029,7 @@
     </row>
     <row r="20" spans="1:18" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C20" s="10">
         <v>2</v>
@@ -1947,7 +2039,7 @@
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G20" s="10">
         <v>2.5</v>
@@ -1957,7 +2049,7 @@
       </c>
       <c r="I20" s="2"/>
       <c r="J20" s="28" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K20" s="29">
         <v>1.2</v>
@@ -1974,7 +2066,7 @@
     </row>
     <row r="21" spans="1:18" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C21" s="10">
         <v>1.5</v>
@@ -1984,7 +2076,7 @@
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G21" s="10">
         <v>1</v>
@@ -1994,7 +2086,7 @@
       </c>
       <c r="I21" s="2"/>
       <c r="J21" s="9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="K21" s="10">
         <v>2</v>
@@ -2010,7 +2102,7 @@
     </row>
     <row r="22" spans="1:18" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C22" s="14">
         <v>1</v>
@@ -2020,7 +2112,7 @@
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="16" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G22" s="17">
         <f>+G14+G15+G16+G17+G18+G19+G20+G21</f>
@@ -2032,7 +2124,7 @@
       </c>
       <c r="I22" s="2"/>
       <c r="J22" s="33" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K22" s="34">
         <v>1</v>
@@ -2047,7 +2139,7 @@
     </row>
     <row r="23" spans="1:18" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C23" s="17">
         <f>C16+C17+C18+C19+C20+C21+C22</f>
@@ -2063,7 +2155,7 @@
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K23" s="17">
         <f>K19+K20+K21+K22</f>
@@ -2100,41 +2192,41 @@
         <f>C15+C23</f>
         <v>30</v>
       </c>
-      <c r="C25" s="43">
+      <c r="C25" s="48">
         <f>(D15*C15+D23*C23)/B25</f>
         <v>15.526500000000002</v>
       </c>
-      <c r="D25" s="44"/>
+      <c r="D25" s="49"/>
       <c r="E25" s="2"/>
       <c r="F25" s="37">
         <f>G13+G22</f>
         <v>30</v>
       </c>
-      <c r="G25" s="43">
+      <c r="G25" s="48">
         <f>(H13*G13+H22*G22)/F25</f>
         <v>13.769583333333333</v>
       </c>
-      <c r="H25" s="44"/>
+      <c r="H25" s="49"/>
       <c r="I25" s="2"/>
       <c r="J25" s="37">
         <f>K11+K18+K23</f>
         <v>30</v>
       </c>
-      <c r="K25" s="39">
+      <c r="K25" s="44">
         <f>(L11*K11+L18*K18+L23*K23)/(K23+K18+K11)</f>
         <v>13.659333333333333</v>
       </c>
-      <c r="L25" s="41"/>
+      <c r="L25" s="46"/>
       <c r="M25" s="2"/>
       <c r="N25" s="37">
-        <f>O11+O16+O22+O17</f>
+        <f>O10+O16+O22+O17</f>
         <v>30</v>
       </c>
-      <c r="O25" s="39">
-        <f>(P11*O11+P16*O16)/(O11+O18)</f>
-        <v>18</v>
-      </c>
-      <c r="P25" s="41"/>
+      <c r="O25" s="44">
+        <f>(P10*O10+P16*O16+P17*O17)/(O10+O16+O17)</f>
+        <v>12.333166666666667</v>
+      </c>
+      <c r="P25" s="46"/>
     </row>
     <row r="26" spans="1:18" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="2"/>
@@ -2155,27 +2247,27 @@
     </row>
     <row r="27" spans="1:18" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
-      <c r="B27" s="39">
+      <c r="B27" s="44">
         <f>(C25+G25)/2</f>
         <v>14.648041666666668</v>
       </c>
-      <c r="C27" s="42"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="42"/>
-      <c r="F27" s="42"/>
-      <c r="G27" s="42"/>
-      <c r="H27" s="41"/>
+      <c r="C27" s="47"/>
+      <c r="D27" s="47"/>
+      <c r="E27" s="47"/>
+      <c r="F27" s="47"/>
+      <c r="G27" s="47"/>
+      <c r="H27" s="46"/>
       <c r="I27" s="2"/>
-      <c r="J27" s="39">
+      <c r="J27" s="44">
         <f>(K25+O25)/2</f>
-        <v>15.829666666666666</v>
-      </c>
-      <c r="K27" s="42"/>
-      <c r="L27" s="42"/>
-      <c r="M27" s="42"/>
-      <c r="N27" s="42"/>
-      <c r="O27" s="42"/>
-      <c r="P27" s="41"/>
+        <v>12.99625</v>
+      </c>
+      <c r="K27" s="47"/>
+      <c r="L27" s="47"/>
+      <c r="M27" s="47"/>
+      <c r="N27" s="47"/>
+      <c r="O27" s="47"/>
+      <c r="P27" s="46"/>
     </row>
     <row r="28" spans="1:18" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
@@ -2196,24 +2288,24 @@
     </row>
     <row r="29" spans="1:18" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
-      <c r="B29" s="39">
+      <c r="B29" s="44">
         <f>(B27+J27)/2</f>
-        <v>15.238854166666666</v>
-      </c>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="40"/>
-      <c r="G29" s="40"/>
-      <c r="H29" s="40"/>
-      <c r="I29" s="40"/>
-      <c r="J29" s="40"/>
-      <c r="K29" s="40"/>
-      <c r="L29" s="40"/>
-      <c r="M29" s="40"/>
-      <c r="N29" s="40"/>
-      <c r="O29" s="40"/>
-      <c r="P29" s="40"/>
+        <v>13.822145833333334</v>
+      </c>
+      <c r="C29" s="45"/>
+      <c r="D29" s="45"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="45"/>
+      <c r="G29" s="45"/>
+      <c r="H29" s="45"/>
+      <c r="I29" s="45"/>
+      <c r="J29" s="45"/>
+      <c r="K29" s="45"/>
+      <c r="L29" s="45"/>
+      <c r="M29" s="45"/>
+      <c r="N29" s="45"/>
+      <c r="O29" s="45"/>
+      <c r="P29" s="45"/>
       <c r="Q29" s="38"/>
     </row>
     <row r="30" spans="1:18" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3244,12 +3336,12 @@
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D14 D16:D22 H3:H12 H14:H21 P17 B29:P29 B27:H27 J27:P27 O25:P25 K25:L25 G25:H25 C25:D25 L3:L10 L12:L17 L19:L22 P3:P10 P12:P15">
+  <conditionalFormatting sqref="D3:D14 D16:D22 H3:H12 H14:H21 P17 B29:P29 B27:H27 J27:P27 O25:P25 K25:L25 G25:H25 C25:D25 L3:L10 L12:L17 L19:L22 P3:P9 P11:P15">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D14 D16:D22 H3:H12 H14:H21 P17 B29:P29 B27:H27 J27:P27 O25:P25 K25:L25 G25:H25 C25:D25 L3:L10 L12:L17 L19:L22 P3:P10 P12:P15">
+  <conditionalFormatting sqref="D3:D14 D16:D22 H3:H12 H14:H21 P17 B29:P29 B27:H27 J27:P27 O25:P25 K25:L25 G25:H25 C25:D25 L3:L10 L12:L17 L19:L22 P3:P9 P11:P15">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>10</formula>
     </cfRule>

</xml_diff>